<commit_message>
Modified model training and saved new models.
</commit_message>
<xml_diff>
--- a/classification/data/best_classifiers_config.xlsx
+++ b/classification/data/best_classifiers_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="460" windowWidth="51240" windowHeight="27220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +118,22 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,8 +153,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -150,7 +172,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -472,15 +500,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="50" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" customWidth="1"/>
@@ -810,6 +840,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>